<commit_message>
Correcciones al código y documentos
</commit_message>
<xml_diff>
--- a/Desarrollo/Proyecto SuperShop/Manuales/Gestión/SS-CP.xlsx
+++ b/Desarrollo/Proyecto SuperShop/Manuales/Gestión/SS-CP.xlsx
@@ -126,7 +126,7 @@
     <t xml:space="preserve">Especificar Requisitos del Software 1:  </t>
   </si>
   <si>
-    <t>Sistema de logeo para poder ingresar al almacén</t>
+    <t>Sistema de logeo</t>
   </si>
   <si>
     <t>SS-SDL.DOCX</t>
@@ -138,10 +138,10 @@
     <t xml:space="preserve">Especificar Requisito del Software 2: </t>
   </si>
   <si>
-    <t>Añadir productos al inventario del programa</t>
-  </si>
-  <si>
-    <t>SS-ANA.DOCX</t>
+    <t>Añadir productos</t>
+  </si>
+  <si>
+    <t>SS-AP.DOCX</t>
   </si>
   <si>
     <t>Santa Cruz E. (T)</t>
@@ -150,10 +150,10 @@
     <t xml:space="preserve">Especificar Requisito del Software 3: </t>
   </si>
   <si>
-    <t>Eliminar productos al inventario del programa</t>
-  </si>
-  <si>
-    <t>SS-ELI.DOCX</t>
+    <t>Eliminar productos del inventario</t>
+  </si>
+  <si>
+    <t>SS-EPI.DOCX</t>
   </si>
   <si>
     <t>Caballero Meza O./FE(FrontEnd)</t>
@@ -165,7 +165,7 @@
     <t>Modificar productos del inventario</t>
   </si>
   <si>
-    <t>SS-MOD.DOCX</t>
+    <t>SS-MPI.DOCX</t>
   </si>
   <si>
     <t>Especificar Requisito del Software 5:</t>
@@ -174,7 +174,7 @@
     <t>Generar reporte del inventario</t>
   </si>
   <si>
-    <t>SS-GRPI.DOCX</t>
+    <t>SS-GRI.PDF</t>
   </si>
   <si>
     <t>Canales Borda G. /Desarrollador Back-End (DB), T</t>
@@ -321,7 +321,7 @@
     <t>Documento de Testeo de Funciones</t>
   </si>
   <si>
-    <t>SS-TEF.DOCX</t>
+    <t>SS-DTEF.DOCX</t>
   </si>
   <si>
     <t>Canales Borda G. (T), Santa Cruz E. (T), Rojas. P(QA)</t>
@@ -333,7 +333,7 @@
     <t xml:space="preserve">Documento de Pruebas Unitarios </t>
   </si>
   <si>
-    <t>SS-PU.DOCX</t>
+    <t>SS-DPU.DOCX</t>
   </si>
   <si>
     <t>SS-RDS2.DOCX</t>
@@ -1783,7 +1783,7 @@
         <v>45027.0</v>
       </c>
       <c r="G16" s="26">
-        <v>45073.0</v>
+        <v>45094.0</v>
       </c>
       <c r="H16" s="27">
         <v>0.0</v>
@@ -1865,7 +1865,7 @@
         <v>45042.0</v>
       </c>
       <c r="H19" s="40">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I19" s="28"/>
       <c r="J19" s="31"/>
@@ -1892,7 +1892,7 @@
         <v>45042.0</v>
       </c>
       <c r="H20" s="40">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I20" s="28"/>
       <c r="J20" s="31"/>
@@ -1918,8 +1918,8 @@
       <c r="G21" s="26">
         <v>45042.0</v>
       </c>
-      <c r="H21" s="27">
-        <v>1.0</v>
+      <c r="H21" s="40">
+        <v>0.5</v>
       </c>
       <c r="I21" s="28"/>
       <c r="J21" s="31"/>
@@ -1946,7 +1946,7 @@
         <v>45042.0</v>
       </c>
       <c r="H22" s="40">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I22" s="28"/>
       <c r="J22" s="31"/>
@@ -1974,8 +1974,8 @@
       <c r="G23" s="26">
         <v>45044.0</v>
       </c>
-      <c r="H23" s="27">
-        <v>1.0</v>
+      <c r="H23" s="40">
+        <v>0.5</v>
       </c>
       <c r="I23" s="28"/>
       <c r="J23" s="31"/>
@@ -2305,8 +2305,8 @@
       <c r="G36" s="26">
         <v>45070.0</v>
       </c>
-      <c r="H36" s="27">
-        <v>0.0</v>
+      <c r="H36" s="40">
+        <v>1.0</v>
       </c>
       <c r="I36" s="28" t="s">
         <v>108</v>
@@ -2334,8 +2334,8 @@
       <c r="G37" s="26">
         <v>45070.0</v>
       </c>
-      <c r="H37" s="27">
-        <v>0.0</v>
+      <c r="H37" s="40">
+        <v>1.0</v>
       </c>
       <c r="J37" s="31"/>
       <c r="K37" s="5"/>
@@ -2375,10 +2375,10 @@
         <v>91</v>
       </c>
       <c r="F39" s="26">
-        <v>45064.0</v>
+        <v>45070.0</v>
       </c>
       <c r="G39" s="26">
-        <v>45071.0</v>
+        <v>45078.0</v>
       </c>
       <c r="H39" s="27">
         <v>0.0</v>
@@ -2402,10 +2402,10 @@
         <v>43</v>
       </c>
       <c r="F40" s="26">
-        <v>45064.0</v>
+        <v>45070.0</v>
       </c>
       <c r="G40" s="26">
-        <v>45071.0</v>
+        <v>45078.0</v>
       </c>
       <c r="H40" s="27">
         <v>0.0</v>
@@ -2428,10 +2428,10 @@
         <v>99</v>
       </c>
       <c r="F41" s="26">
-        <v>45064.0</v>
+        <v>45070.0</v>
       </c>
       <c r="G41" s="26">
-        <v>45071.0</v>
+        <v>45078.0</v>
       </c>
       <c r="H41" s="27">
         <v>0.0</v>
@@ -2454,10 +2454,10 @@
         <v>63</v>
       </c>
       <c r="F42" s="26">
-        <v>45064.0</v>
+        <v>45070.0</v>
       </c>
       <c r="G42" s="26">
-        <v>45071.0</v>
+        <v>45078.0</v>
       </c>
       <c r="H42" s="27">
         <v>0.0</v>

</xml_diff>

<commit_message>
Agregados los documentos de la Linea Base 3
</commit_message>
<xml_diff>
--- a/Desarrollo/Proyecto SuperShop/Manuales/Gestión/SS-CP.xlsx
+++ b/Desarrollo/Proyecto SuperShop/Manuales/Gestión/SS-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akcel\OneDrive\Escritorio\ae\sistema-ecommerce\Desarrollo\Proyecto SuperShop\Manuales\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akcel\OneDrive\Escritorio\repoasubir\sistema-ecommerce\Desarrollo\Proyecto SuperShop\Manuales\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879BD96A-234F-47BF-BCAC-AFC30B501F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1D96B3-64B2-494A-AB4F-8F32944045D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1255,22 +1255,22 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1497,7 +1497,7 @@
   <dimension ref="A1:K1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1513,23 +1513,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="78"/>
+      <c r="C2" s="74"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -1641,7 +1641,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="75" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="18" t="s">
@@ -1669,7 +1669,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A11" s="72"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="18" t="s">
         <v>20</v>
       </c>
@@ -1691,13 +1691,13 @@
       <c r="H11" s="23">
         <v>1</v>
       </c>
-      <c r="I11" s="74" t="s">
+      <c r="I11" s="78" t="s">
         <v>22</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="72"/>
+      <c r="A12" s="76"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -1710,12 +1710,12 @@
       <c r="H12" s="23">
         <v>1</v>
       </c>
-      <c r="I12" s="75"/>
+      <c r="I12" s="72"/>
       <c r="J12" s="26"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="72"/>
+      <c r="A13" s="76"/>
       <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
@@ -1737,14 +1737,14 @@
       <c r="H13" s="23">
         <v>1</v>
       </c>
-      <c r="I13" s="74" t="s">
+      <c r="I13" s="78" t="s">
         <v>27</v>
       </c>
       <c r="J13" s="26"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="72"/>
+      <c r="A14" s="76"/>
       <c r="B14" s="18" t="s">
         <v>28</v>
       </c>
@@ -1760,11 +1760,11 @@
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="23"/>
-      <c r="I14" s="75"/>
+      <c r="I14" s="72"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="72"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="18" t="s">
         <v>31</v>
       </c>
@@ -1786,11 +1786,11 @@
       <c r="H15" s="23">
         <v>1</v>
       </c>
-      <c r="I15" s="75"/>
+      <c r="I15" s="72"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A16" s="72"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="18" t="s">
         <v>33</v>
       </c>
@@ -1812,12 +1812,12 @@
       <c r="H16" s="23">
         <v>0</v>
       </c>
-      <c r="I16" s="75"/>
+      <c r="I16" s="72"/>
       <c r="J16" s="26"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="72"/>
+      <c r="A17" s="76"/>
       <c r="B17" s="18" t="s">
         <v>36</v>
       </c>
@@ -1839,12 +1839,12 @@
       <c r="H17" s="23">
         <v>1</v>
       </c>
-      <c r="I17" s="75"/>
+      <c r="I17" s="72"/>
       <c r="J17" s="26"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A18" s="72"/>
+      <c r="A18" s="76"/>
       <c r="B18" s="18" t="s">
         <v>40</v>
       </c>
@@ -1871,7 +1871,7 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A19" s="72"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="18" t="s">
         <v>44</v>
       </c>
@@ -1898,7 +1898,7 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="72"/>
+      <c r="A20" s="76"/>
       <c r="B20" s="18" t="s">
         <v>48</v>
       </c>
@@ -1925,7 +1925,7 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="72"/>
+      <c r="A21" s="76"/>
       <c r="B21" s="18" t="s">
         <v>51</v>
       </c>
@@ -1952,7 +1952,7 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="73"/>
+      <c r="A22" s="77"/>
       <c r="B22" s="18" t="s">
         <v>55</v>
       </c>
@@ -1979,7 +1979,7 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="79" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="18" t="s">
@@ -2008,7 +2008,7 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="72"/>
+      <c r="A24" s="76"/>
       <c r="B24" s="18" t="s">
         <v>64</v>
       </c>
@@ -2030,14 +2030,14 @@
       <c r="H24" s="23">
         <v>1</v>
       </c>
-      <c r="I24" s="74" t="s">
+      <c r="I24" s="78" t="s">
         <v>68</v>
       </c>
       <c r="J24" s="26"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A25" s="72"/>
+      <c r="A25" s="76"/>
       <c r="B25" s="18" t="s">
         <v>69</v>
       </c>
@@ -2059,12 +2059,12 @@
       <c r="H25" s="23">
         <v>1</v>
       </c>
-      <c r="I25" s="75"/>
+      <c r="I25" s="72"/>
       <c r="J25" s="26"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="72"/>
+      <c r="A26" s="76"/>
       <c r="B26" s="33" t="s">
         <v>72</v>
       </c>
@@ -2086,12 +2086,12 @@
       <c r="H26" s="23">
         <v>1</v>
       </c>
-      <c r="I26" s="75"/>
+      <c r="I26" s="72"/>
       <c r="J26" s="26"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="72"/>
+      <c r="A27" s="76"/>
       <c r="B27" s="33" t="s">
         <v>76</v>
       </c>
@@ -2108,7 +2108,7 @@
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="72"/>
+      <c r="A28" s="76"/>
       <c r="B28" s="18" t="s">
         <v>77</v>
       </c>
@@ -2130,14 +2130,14 @@
       <c r="H28" s="23">
         <v>1</v>
       </c>
-      <c r="I28" s="74" t="s">
+      <c r="I28" s="78" t="s">
         <v>81</v>
       </c>
       <c r="J28" s="26"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A29" s="73"/>
+      <c r="A29" s="77"/>
       <c r="B29" s="18" t="s">
         <v>82</v>
       </c>
@@ -2159,7 +2159,7 @@
       <c r="H29" s="23">
         <v>1</v>
       </c>
-      <c r="I29" s="75"/>
+      <c r="I29" s="72"/>
       <c r="J29" s="26"/>
       <c r="K29" s="2"/>
     </row>
@@ -2178,10 +2178,10 @@
         <v>45046</v>
       </c>
       <c r="H30" s="40"/>
-      <c r="I30" s="75"/>
+      <c r="I30" s="72"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="79" t="s">
         <v>87</v>
       </c>
       <c r="B31" s="41" t="s">
@@ -2205,14 +2205,14 @@
       <c r="H31" s="42">
         <v>0</v>
       </c>
-      <c r="I31" s="74" t="s">
+      <c r="I31" s="78" t="s">
         <v>92</v>
       </c>
       <c r="J31" s="26"/>
       <c r="K31" s="43"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A32" s="72"/>
+      <c r="A32" s="76"/>
       <c r="B32" s="41" t="s">
         <v>93</v>
       </c>
@@ -2234,12 +2234,12 @@
       <c r="H32" s="44">
         <v>1</v>
       </c>
-      <c r="I32" s="75"/>
+      <c r="I32" s="72"/>
       <c r="J32" s="26"/>
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A33" s="72"/>
+      <c r="A33" s="76"/>
       <c r="B33" s="45" t="s">
         <v>96</v>
       </c>
@@ -2261,12 +2261,12 @@
       <c r="H33" s="42">
         <v>1</v>
       </c>
-      <c r="I33" s="75"/>
+      <c r="I33" s="72"/>
       <c r="J33" s="26"/>
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="72"/>
+      <c r="A34" s="76"/>
       <c r="B34" s="18" t="s">
         <v>100</v>
       </c>
@@ -2288,12 +2288,12 @@
       <c r="H34" s="44">
         <v>1</v>
       </c>
-      <c r="I34" s="75"/>
+      <c r="I34" s="72"/>
       <c r="J34" s="26"/>
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="72"/>
+      <c r="A35" s="76"/>
       <c r="B35" s="18" t="s">
         <v>104</v>
       </c>
@@ -2315,12 +2315,12 @@
       <c r="H35" s="23">
         <v>1</v>
       </c>
-      <c r="I35" s="75"/>
+      <c r="I35" s="72"/>
       <c r="J35" s="26"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="72"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="18" t="s">
         <v>77</v>
       </c>
@@ -2342,14 +2342,14 @@
       <c r="H36" s="23">
         <v>1</v>
       </c>
-      <c r="I36" s="74" t="s">
+      <c r="I36" s="78" t="s">
         <v>108</v>
       </c>
       <c r="J36" s="26"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A37" s="73"/>
+      <c r="A37" s="77"/>
       <c r="B37" s="18" t="s">
         <v>82</v>
       </c>
@@ -2371,7 +2371,7 @@
       <c r="H37" s="23">
         <v>1</v>
       </c>
-      <c r="I37" s="75"/>
+      <c r="I37" s="72"/>
       <c r="J37" s="26"/>
       <c r="K37" s="2"/>
     </row>
@@ -2392,10 +2392,10 @@
         <v>45070</v>
       </c>
       <c r="H38" s="49"/>
-      <c r="I38" s="75"/>
+      <c r="I38" s="72"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="71" t="s">
+      <c r="A39" s="79" t="s">
         <v>113</v>
       </c>
       <c r="B39" s="41" t="s">
@@ -2419,12 +2419,12 @@
       <c r="H39" s="23">
         <v>0</v>
       </c>
-      <c r="I39" s="74"/>
+      <c r="I39" s="78"/>
       <c r="J39" s="26"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A40" s="72"/>
+      <c r="A40" s="76"/>
       <c r="B40" s="41" t="s">
         <v>115</v>
       </c>
@@ -2446,12 +2446,12 @@
       <c r="H40" s="23">
         <v>1</v>
       </c>
-      <c r="I40" s="75"/>
+      <c r="I40" s="72"/>
       <c r="J40" s="26"/>
       <c r="K40" s="2"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A41" s="72"/>
+      <c r="A41" s="76"/>
       <c r="B41" s="45" t="s">
         <v>117</v>
       </c>
@@ -2473,12 +2473,12 @@
       <c r="H41" s="23">
         <v>1</v>
       </c>
-      <c r="I41" s="75"/>
+      <c r="I41" s="72"/>
       <c r="J41" s="26"/>
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A42" s="72"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="18" t="s">
         <v>119</v>
       </c>
@@ -2500,12 +2500,12 @@
       <c r="H42" s="23">
         <v>0</v>
       </c>
-      <c r="I42" s="75"/>
+      <c r="I42" s="72"/>
       <c r="J42" s="26"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A43" s="72"/>
+      <c r="A43" s="76"/>
       <c r="B43" s="18" t="s">
         <v>121</v>
       </c>
@@ -2525,16 +2525,16 @@
         <v>45093</v>
       </c>
       <c r="H43" s="23">
-        <v>0</v>
-      </c>
-      <c r="I43" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" s="78" t="s">
         <v>124</v>
       </c>
       <c r="J43" s="26"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A44" s="72"/>
+      <c r="A44" s="76"/>
       <c r="B44" s="18" t="s">
         <v>77</v>
       </c>
@@ -2554,14 +2554,14 @@
         <v>45093</v>
       </c>
       <c r="H44" s="23">
-        <v>0</v>
-      </c>
-      <c r="I44" s="75"/>
+        <v>1</v>
+      </c>
+      <c r="I44" s="72"/>
       <c r="J44" s="26"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="27" customHeight="1">
-      <c r="A45" s="72"/>
+      <c r="A45" s="76"/>
       <c r="B45" s="18" t="s">
         <v>82</v>
       </c>
@@ -2581,16 +2581,16 @@
         <v>45098</v>
       </c>
       <c r="H45" s="23">
-        <v>0</v>
-      </c>
-      <c r="I45" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="I45" s="78" t="s">
         <v>128</v>
       </c>
       <c r="J45" s="26"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A46" s="72"/>
+      <c r="A46" s="76"/>
       <c r="B46" s="18" t="s">
         <v>129</v>
       </c>
@@ -2610,14 +2610,14 @@
         <v>45094</v>
       </c>
       <c r="H46" s="23">
-        <v>0</v>
-      </c>
-      <c r="I46" s="75"/>
+        <v>1</v>
+      </c>
+      <c r="I46" s="72"/>
       <c r="J46" s="26"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A47" s="73"/>
+      <c r="A47" s="77"/>
       <c r="B47" s="50" t="s">
         <v>132</v>
       </c>
@@ -2639,7 +2639,7 @@
       <c r="H47" s="23">
         <v>0</v>
       </c>
-      <c r="I47" s="75"/>
+      <c r="I47" s="72"/>
       <c r="J47" s="26"/>
       <c r="K47" s="2"/>
     </row>
@@ -2660,7 +2660,7 @@
         <v>45098</v>
       </c>
       <c r="H48" s="57"/>
-      <c r="I48" s="75"/>
+      <c r="I48" s="72"/>
     </row>
     <row r="49" spans="2:8" ht="15.75" customHeight="1">
       <c r="B49" s="58"/>
@@ -4424,11 +4424,6 @@
     <row r="1003" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A10:A22"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I17"/>
     <mergeCell ref="A23:A29"/>
     <mergeCell ref="A31:A37"/>
     <mergeCell ref="A39:A47"/>
@@ -4439,6 +4434,11 @@
     <mergeCell ref="I45:I48"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="I28:I30"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A10:A22"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
@@ -4473,7 +4473,7 @@
       <c r="B3" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="78"/>
+      <c r="C3" s="74"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
       <c r="B4" s="62" t="s">

</xml_diff>

<commit_message>
Subida las solicitudes de cambio
</commit_message>
<xml_diff>
--- a/Desarrollo/Proyecto SuperShop/Manuales/Gestión/SS-CP.xlsx
+++ b/Desarrollo/Proyecto SuperShop/Manuales/Gestión/SS-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akcel\OneDrive\Escritorio\repoasubir\sistema-ecommerce\Desarrollo\Proyecto SuperShop\Manuales\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akcel\OneDrive\Escritorio\Nueva carpeta (3)\sistema-ecommerce\Desarrollo\Proyecto SuperShop\Manuales\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1D96B3-64B2-494A-AB4F-8F32944045D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88CE1FF-7399-4463-9B3B-5D9FAE8279DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1255,22 +1255,22 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1496,8 +1496,8 @@
   </sheetPr>
   <dimension ref="A1:K1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1513,23 +1513,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="74"/>
+      <c r="C2" s="78"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -1641,7 +1641,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="79" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="18" t="s">
@@ -1669,7 +1669,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A11" s="76"/>
+      <c r="A11" s="72"/>
       <c r="B11" s="18" t="s">
         <v>20</v>
       </c>
@@ -1691,13 +1691,13 @@
       <c r="H11" s="23">
         <v>1</v>
       </c>
-      <c r="I11" s="78" t="s">
+      <c r="I11" s="74" t="s">
         <v>22</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="76"/>
+      <c r="A12" s="72"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -1710,12 +1710,12 @@
       <c r="H12" s="23">
         <v>1</v>
       </c>
-      <c r="I12" s="72"/>
+      <c r="I12" s="75"/>
       <c r="J12" s="26"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="76"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
@@ -1737,14 +1737,14 @@
       <c r="H13" s="23">
         <v>1</v>
       </c>
-      <c r="I13" s="78" t="s">
+      <c r="I13" s="74" t="s">
         <v>27</v>
       </c>
       <c r="J13" s="26"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="76"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="18" t="s">
         <v>28</v>
       </c>
@@ -1760,11 +1760,11 @@
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="23"/>
-      <c r="I14" s="72"/>
+      <c r="I14" s="75"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="76"/>
+      <c r="A15" s="72"/>
       <c r="B15" s="18" t="s">
         <v>31</v>
       </c>
@@ -1786,11 +1786,11 @@
       <c r="H15" s="23">
         <v>1</v>
       </c>
-      <c r="I15" s="72"/>
+      <c r="I15" s="75"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A16" s="76"/>
+      <c r="A16" s="72"/>
       <c r="B16" s="18" t="s">
         <v>33</v>
       </c>
@@ -1810,14 +1810,14 @@
         <v>45094</v>
       </c>
       <c r="H16" s="23">
-        <v>0</v>
-      </c>
-      <c r="I16" s="72"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="75"/>
       <c r="J16" s="26"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="76"/>
+      <c r="A17" s="72"/>
       <c r="B17" s="18" t="s">
         <v>36</v>
       </c>
@@ -1839,12 +1839,12 @@
       <c r="H17" s="23">
         <v>1</v>
       </c>
-      <c r="I17" s="72"/>
+      <c r="I17" s="75"/>
       <c r="J17" s="26"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A18" s="76"/>
+      <c r="A18" s="72"/>
       <c r="B18" s="18" t="s">
         <v>40</v>
       </c>
@@ -1871,7 +1871,7 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A19" s="76"/>
+      <c r="A19" s="72"/>
       <c r="B19" s="18" t="s">
         <v>44</v>
       </c>
@@ -1898,7 +1898,7 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="76"/>
+      <c r="A20" s="72"/>
       <c r="B20" s="18" t="s">
         <v>48</v>
       </c>
@@ -1925,7 +1925,7 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="76"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="18" t="s">
         <v>51</v>
       </c>
@@ -1952,7 +1952,7 @@
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="77"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="18" t="s">
         <v>55</v>
       </c>
@@ -1979,7 +1979,7 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="71" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="18" t="s">
@@ -2008,7 +2008,7 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="76"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="18" t="s">
         <v>64</v>
       </c>
@@ -2030,14 +2030,14 @@
       <c r="H24" s="23">
         <v>1</v>
       </c>
-      <c r="I24" s="78" t="s">
+      <c r="I24" s="74" t="s">
         <v>68</v>
       </c>
       <c r="J24" s="26"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A25" s="76"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="18" t="s">
         <v>69</v>
       </c>
@@ -2059,12 +2059,12 @@
       <c r="H25" s="23">
         <v>1</v>
       </c>
-      <c r="I25" s="72"/>
+      <c r="I25" s="75"/>
       <c r="J25" s="26"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="76"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="33" t="s">
         <v>72</v>
       </c>
@@ -2086,12 +2086,12 @@
       <c r="H26" s="23">
         <v>1</v>
       </c>
-      <c r="I26" s="72"/>
+      <c r="I26" s="75"/>
       <c r="J26" s="26"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="76"/>
+      <c r="A27" s="72"/>
       <c r="B27" s="33" t="s">
         <v>76</v>
       </c>
@@ -2108,7 +2108,7 @@
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="76"/>
+      <c r="A28" s="72"/>
       <c r="B28" s="18" t="s">
         <v>77</v>
       </c>
@@ -2130,14 +2130,14 @@
       <c r="H28" s="23">
         <v>1</v>
       </c>
-      <c r="I28" s="78" t="s">
+      <c r="I28" s="74" t="s">
         <v>81</v>
       </c>
       <c r="J28" s="26"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="24.75" customHeight="1">
-      <c r="A29" s="77"/>
+      <c r="A29" s="73"/>
       <c r="B29" s="18" t="s">
         <v>82</v>
       </c>
@@ -2159,7 +2159,7 @@
       <c r="H29" s="23">
         <v>1</v>
       </c>
-      <c r="I29" s="72"/>
+      <c r="I29" s="75"/>
       <c r="J29" s="26"/>
       <c r="K29" s="2"/>
     </row>
@@ -2178,10 +2178,10 @@
         <v>45046</v>
       </c>
       <c r="H30" s="40"/>
-      <c r="I30" s="72"/>
+      <c r="I30" s="75"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="71" t="s">
         <v>87</v>
       </c>
       <c r="B31" s="41" t="s">
@@ -2205,14 +2205,14 @@
       <c r="H31" s="42">
         <v>0</v>
       </c>
-      <c r="I31" s="78" t="s">
+      <c r="I31" s="74" t="s">
         <v>92</v>
       </c>
       <c r="J31" s="26"/>
       <c r="K31" s="43"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A32" s="76"/>
+      <c r="A32" s="72"/>
       <c r="B32" s="41" t="s">
         <v>93</v>
       </c>
@@ -2234,12 +2234,12 @@
       <c r="H32" s="44">
         <v>1</v>
       </c>
-      <c r="I32" s="72"/>
+      <c r="I32" s="75"/>
       <c r="J32" s="26"/>
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A33" s="76"/>
+      <c r="A33" s="72"/>
       <c r="B33" s="45" t="s">
         <v>96</v>
       </c>
@@ -2261,12 +2261,12 @@
       <c r="H33" s="42">
         <v>1</v>
       </c>
-      <c r="I33" s="72"/>
+      <c r="I33" s="75"/>
       <c r="J33" s="26"/>
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="76"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="18" t="s">
         <v>100</v>
       </c>
@@ -2288,12 +2288,12 @@
       <c r="H34" s="44">
         <v>1</v>
       </c>
-      <c r="I34" s="72"/>
+      <c r="I34" s="75"/>
       <c r="J34" s="26"/>
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="76"/>
+      <c r="A35" s="72"/>
       <c r="B35" s="18" t="s">
         <v>104</v>
       </c>
@@ -2315,12 +2315,12 @@
       <c r="H35" s="23">
         <v>1</v>
       </c>
-      <c r="I35" s="72"/>
+      <c r="I35" s="75"/>
       <c r="J35" s="26"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="76"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="18" t="s">
         <v>77</v>
       </c>
@@ -2342,14 +2342,14 @@
       <c r="H36" s="23">
         <v>1</v>
       </c>
-      <c r="I36" s="78" t="s">
+      <c r="I36" s="74" t="s">
         <v>108</v>
       </c>
       <c r="J36" s="26"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="27.75" customHeight="1">
-      <c r="A37" s="77"/>
+      <c r="A37" s="73"/>
       <c r="B37" s="18" t="s">
         <v>82</v>
       </c>
@@ -2371,7 +2371,7 @@
       <c r="H37" s="23">
         <v>1</v>
       </c>
-      <c r="I37" s="72"/>
+      <c r="I37" s="75"/>
       <c r="J37" s="26"/>
       <c r="K37" s="2"/>
     </row>
@@ -2392,10 +2392,10 @@
         <v>45070</v>
       </c>
       <c r="H38" s="49"/>
-      <c r="I38" s="72"/>
+      <c r="I38" s="75"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="79" t="s">
+      <c r="A39" s="71" t="s">
         <v>113</v>
       </c>
       <c r="B39" s="41" t="s">
@@ -2419,12 +2419,12 @@
       <c r="H39" s="23">
         <v>0</v>
       </c>
-      <c r="I39" s="78"/>
+      <c r="I39" s="74"/>
       <c r="J39" s="26"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A40" s="76"/>
+      <c r="A40" s="72"/>
       <c r="B40" s="41" t="s">
         <v>115</v>
       </c>
@@ -2446,12 +2446,12 @@
       <c r="H40" s="23">
         <v>1</v>
       </c>
-      <c r="I40" s="72"/>
+      <c r="I40" s="75"/>
       <c r="J40" s="26"/>
       <c r="K40" s="2"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A41" s="76"/>
+      <c r="A41" s="72"/>
       <c r="B41" s="45" t="s">
         <v>117</v>
       </c>
@@ -2473,12 +2473,12 @@
       <c r="H41" s="23">
         <v>1</v>
       </c>
-      <c r="I41" s="72"/>
+      <c r="I41" s="75"/>
       <c r="J41" s="26"/>
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A42" s="76"/>
+      <c r="A42" s="72"/>
       <c r="B42" s="18" t="s">
         <v>119</v>
       </c>
@@ -2500,12 +2500,12 @@
       <c r="H42" s="23">
         <v>0</v>
       </c>
-      <c r="I42" s="72"/>
+      <c r="I42" s="75"/>
       <c r="J42" s="26"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A43" s="76"/>
+      <c r="A43" s="72"/>
       <c r="B43" s="18" t="s">
         <v>121</v>
       </c>
@@ -2527,14 +2527,14 @@
       <c r="H43" s="23">
         <v>1</v>
       </c>
-      <c r="I43" s="78" t="s">
+      <c r="I43" s="74" t="s">
         <v>124</v>
       </c>
       <c r="J43" s="26"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A44" s="76"/>
+      <c r="A44" s="72"/>
       <c r="B44" s="18" t="s">
         <v>77</v>
       </c>
@@ -2556,12 +2556,12 @@
       <c r="H44" s="23">
         <v>1</v>
       </c>
-      <c r="I44" s="72"/>
+      <c r="I44" s="75"/>
       <c r="J44" s="26"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="27" customHeight="1">
-      <c r="A45" s="76"/>
+      <c r="A45" s="72"/>
       <c r="B45" s="18" t="s">
         <v>82</v>
       </c>
@@ -2583,14 +2583,14 @@
       <c r="H45" s="23">
         <v>1</v>
       </c>
-      <c r="I45" s="78" t="s">
+      <c r="I45" s="74" t="s">
         <v>128</v>
       </c>
       <c r="J45" s="26"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A46" s="76"/>
+      <c r="A46" s="72"/>
       <c r="B46" s="18" t="s">
         <v>129</v>
       </c>
@@ -2612,12 +2612,12 @@
       <c r="H46" s="23">
         <v>1</v>
       </c>
-      <c r="I46" s="72"/>
+      <c r="I46" s="75"/>
       <c r="J46" s="26"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A47" s="77"/>
+      <c r="A47" s="73"/>
       <c r="B47" s="50" t="s">
         <v>132</v>
       </c>
@@ -2637,9 +2637,9 @@
         <v>45098</v>
       </c>
       <c r="H47" s="23">
-        <v>0</v>
-      </c>
-      <c r="I47" s="72"/>
+        <v>0.8</v>
+      </c>
+      <c r="I47" s="75"/>
       <c r="J47" s="26"/>
       <c r="K47" s="2"/>
     </row>
@@ -2660,7 +2660,7 @@
         <v>45098</v>
       </c>
       <c r="H48" s="57"/>
-      <c r="I48" s="72"/>
+      <c r="I48" s="75"/>
     </row>
     <row r="49" spans="2:8" ht="15.75" customHeight="1">
       <c r="B49" s="58"/>
@@ -4424,6 +4424,11 @@
     <row r="1003" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A10:A22"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I17"/>
     <mergeCell ref="A23:A29"/>
     <mergeCell ref="A31:A37"/>
     <mergeCell ref="A39:A47"/>
@@ -4434,11 +4439,6 @@
     <mergeCell ref="I45:I48"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="I28:I30"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A10:A22"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
@@ -4473,7 +4473,7 @@
       <c r="B3" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="78"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
       <c r="B4" s="62" t="s">

</xml_diff>